<commit_message>
add the survey script, minor changes in the figure
</commit_message>
<xml_diff>
--- a/data/diamond_pipelines_data.xlsx
+++ b/data/diamond_pipelines_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gxexakis/code/IAM-development-practices/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{982553CE-AAEB-8E40-BF22-5384FB551396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94EEBA79-59B4-274A-8FF8-A20864CB875C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6580" yWindow="500" windowWidth="31820" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="19200" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -717,7 +717,7 @@
     <t>Comments within the code;README files;Word document;Online documentation platform or wiki page (e.g., Read the Docs);All of the above, plus a automated documentation framework</t>
   </si>
   <si>
-    <t>TXT, JSON, or YAML files;Comments on the dataset (e.g., on the top of CSV files);External README files;Documented code that handles the whole input data processing pipeline</t>
+    <t>Comments on the dataset (e.g., on the top of CSV files);External README files;Documented code that handles the whole input data processing pipeline</t>
   </si>
 </sst>
 </file>
@@ -1179,8 +1179,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AW10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+    <sheetView tabSelected="1" topLeftCell="U4" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="X7" sqref="X7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>